<commit_message>
initial file stucture is done
</commit_message>
<xml_diff>
--- a/pricing_summary.xlsx
+++ b/pricing_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,45 +436,115 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SL No</t>
+          <t>Srno</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Instance</t>
+          <t>SQL Type</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cloud SQL Edition</t>
+          <t>No. of Instances</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve">Cloud SQL </t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Database Version</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Instance Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>vCPUs</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>RAM</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>HA/Non-HA</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Datacenter Location</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Storage Amt</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Disk Type</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Backup</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Avg no. of hrs</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Hrs/Min</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Days/Month</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>SUD Price</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>SUD URL</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>One Year Price</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>One Year URL</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Three Year Price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Three Year URL</t>
         </is>
@@ -486,40 +556,70 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.02</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>MySQL</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1.02</v>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$325.14</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiQxNkFBRDlFMy1BNjU0LTQ3MEItOTY1RC0yOEUxRkNFMDAxMkE</t>
-        </is>
-      </c>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$249.08</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiQ5QzYxNEFGOS0xNzEyLTRDQzAtQUU2RC1GNzA2RjFBMTUxNjA</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiQzNkY2RjQwNy1EQ0EzLTQ4OTAtOTFFQS0yN0YwMzRFNkY0ODc</t>
-        </is>
+          <t xml:space="preserve">custom </t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+      <c r="H2" t="n">
+        <v>26</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>$166.93</t>
-        </is>
-      </c>
+          <t>Non-HA</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>asia-south1</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" t="n">
+        <v>730</v>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>$305.93</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQyRTMzMzIzRS0xNTIyLTRGMEQtQUJGRS0xRTQyQ0NDRjA3RUI</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -527,38 +627,92 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>MySQL</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$228.42</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiQ0RENFRjlCRi0zQkQ4LTQyQTMtQTQ2OS02MzkxMUVFN0Y0QjY</t>
-        </is>
-      </c>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>$171.69</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiQ4NEE0MkMwMS1BMjg1LTQ0ODgtODk0Qy1GM0U1QzgxN0I1QkQ</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiQ5RDMyMDVDNS1EOTI1LTRBRjgtQThDOC03RTE2RTVBM0M2RDY</t>
-        </is>
+          <t>STANDARD</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" t="n">
+        <v>15</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>$110.42</t>
+          <t>HA</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>asia-southeast1</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>11</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>600</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>hours</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>$456.58</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>$456.58</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>$456.58</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
         </is>
       </c>
     </row>
@@ -568,38 +722,92 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>MySQL</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$65.00</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiQyNzVDOTkwMi1FOTRELTQyRkMtQUE0Qi1COUQ5RUMwNTdCNkY</t>
-        </is>
-      </c>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$51.67</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiRFNkZBQUZDNi0zODVGLTQzQjgtODlFQS1FMDVCRDU0NzFBMDM</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiQzOUZGMTU0RS03MjM1LTQzQjgtOEZCNC00MEYzODg2RjE5Qzk</t>
-        </is>
+          <t>lightweight</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.75</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$37.27</t>
+          <t>Non-HA</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>asia-southeast1</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N4" t="n">
+        <v>350</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>hours</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>$107.88</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>$107.88</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>$107.88</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
         </is>
       </c>
     </row>
@@ -609,38 +817,84 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
+          <t>PostgreSQL</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>f1-micro</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>HA</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>asia-south1</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
+      </c>
+      <c r="N5" t="n">
+        <v>730</v>
+      </c>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr">
+        <is>
           <t>Invalid price format</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiRDQjUzQjMxQS00MEE3LTRFREItQUNCRi00Qjc4NUFEQzgzMTE</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>Invalid price format</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiQwQzU2M0E3Ri0wMUZELTRERTUtQTZBMS0xNDExMDAyQkMyMUM</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiRBQTlCMjVBRi0wM0FDLTRFNkYtOTlGQy1ERDk2QkM1QzkxNzg</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>Invalid price format</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
         </is>
       </c>
     </row>
@@ -650,40 +904,70 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.02</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>PostgreSQL</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1.02</v>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$157.19</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiQ4RERFMTUzQi1BRjNGLTQ5NTMtQkMzRS04Q0E4MEQ4QjY5ODc</t>
-        </is>
-      </c>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$123.57</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiRERkU2MURDQy0zNEU5LTRCQzYtOTc5Qi0zN0JGMjQ1REQwMTA</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiRGQTg4NEVCNy1DNzM1LTQxRDgtOUIwMy04Q0I1RjA4REQ4ODg</t>
-        </is>
+          <t>STANDARD</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7.5</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>$87.27</t>
-        </is>
-      </c>
+          <t>Non-HA</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>asia-southeast1</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>10</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>730</v>
+      </c>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>$272.01</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQwNUU0QTI5Qi04QkY1LTQ0QzUtOTNCRC1DODZDMDdCRDQzRTk</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -691,38 +975,92 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+          <t>PostgreSQL</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$8.60</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJqTXpJeFltTmhPUzAwTldSbExUUXhNMlV0WVRkbU5DMWtNamRrTWpBNU1USTJNMllRQVE9PRAHGiREMkE5RjQ4Ny00MTJDLTRDMEYtOURCMC04NzU2QUZBRjM2MzQ</t>
-        </is>
-      </c>
+          <t>Enterprise</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$6.52</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE0WXpSak5UUTBOUzB3WldReExUUTBaR1l0WWprMk5DMDBNamczTjJaak9UbGhZVEFRQVE9PRAHGiQwQTYxQzRBMC0wRkFDLTQ3NUItQTM2QS0xN0NCNTI4QTU0QTQ</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1Tnpka09UWTRaaTFrTURGakxUUmxNekV0WWpFeU55MDJNVEJrTXpNMU1XTTNObUVRQVE9PRAHGiQxRjFENUQ4NC00OTdGLTQyRjgtOUZGRC0yQTI2RUM4MkRDMEE</t>
-        </is>
+          <t xml:space="preserve">custom </t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>8</v>
+      </c>
+      <c r="H7" t="n">
+        <v>52</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$4.27</t>
+          <t>Non-HA</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>asia-south2</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>11</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>hours</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>$8.36</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQ3MUNFNDZCRS04Q0JGLTQyRjItOTc2Ni1FNTdEQ0IzNUY3MjA</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>$8.36</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQ3MUNFNDZCRS04Q0JGLTQyRjItOTc2Ni1FNTdEQ0IzNUY3MjA</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>$8.36</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrTmpreU56YzNNQzAyTjJJMkxUUTJZVFF0WVRReU5TMWhZVGN3TjJReFpUUXpOV1VRQVE9PRAHGiQ3MUNFNDZCRS04Q0JGLTQyRjItOTc2Ni1FNTdEQ0IzNUY3MjA</t>
         </is>
       </c>
     </row>

</xml_diff>